<commit_message>
fixed a bug where a TC was being scheduled longer than their max hours per day, added printing the TCs desired hours and scheduled hours within the TC post schedule availability txt file
</commit_message>
<xml_diff>
--- a/ExcelFiles/Summer Availability/Summer2015KellyCondon.xlsx
+++ b/ExcelFiles/Summer Availability/Summer2015KellyCondon.xlsx
@@ -354,7 +354,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +403,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -584,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -641,15 +647,6 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -687,7 +684,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -993,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1014,100 +1023,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
     </row>
     <row r="2" spans="1:15" ht="31.5" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
     </row>
     <row r="9" spans="1:15" ht="15" thickBot="1">
       <c r="A9" s="6"/>
@@ -1118,13 +1127,13 @@
       <c r="N9" s="9"/>
     </row>
     <row r="10" spans="1:15" ht="16" thickTop="1" thickBot="1">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -1135,13 +1144,13 @@
       <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:15" ht="15" thickBot="1">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
@@ -1168,16 +1177,16 @@
       <c r="O12" s="9"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
       <c r="I13" s="9"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
@@ -1187,13 +1196,13 @@
       <c r="O13" s="9"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
       <c r="I14" s="9"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -1203,12 +1212,12 @@
       <c r="O14" s="9"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="32"/>
       <c r="I15" s="9"/>
       <c r="J15" s="10"/>
@@ -1219,15 +1228,15 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="5"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
@@ -1238,19 +1247,19 @@
       <c r="O16" s="10"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
@@ -1308,13 +1317,13 @@
       <c r="A20" s="7">
         <v>0.25</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="51"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="51"/>
       <c r="J20" s="11"/>
       <c r="K20" s="11"/>
       <c r="L20" s="11"/>
@@ -1325,13 +1334,13 @@
       <c r="A21" s="7">
         <v>0.27083333333333331</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="51"/>
       <c r="J21" s="11"/>
       <c r="K21" s="11"/>
       <c r="L21" s="11"/>
@@ -1786,19 +1795,25 @@
       <c r="H57" s="26"/>
     </row>
     <row r="58" spans="1:8" ht="15" thickTop="1">
-      <c r="A58" s="39"/>
+      <c r="A58" s="36"/>
     </row>
     <row r="59" spans="1:8">
-      <c r="A59" s="40"/>
+      <c r="A59" s="37"/>
     </row>
     <row r="60" spans="1:8">
-      <c r="A60" s="40"/>
+      <c r="A60" s="37"/>
     </row>
     <row r="61" spans="1:8">
-      <c r="A61" s="40"/>
+      <c r="A61" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A58:A61"/>
     <mergeCell ref="A7:H7"/>
@@ -1810,12 +1825,6 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="E17:I17"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1844,121 +1853,121 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" ht="31.5" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="14">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="14">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="14">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="14">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="14">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="14">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
       <c r="I8" s="2"/>
       <c r="J8" s="50"/>
       <c r="K8" s="50"/>
@@ -1977,13 +1986,13 @@
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" ht="16" thickTop="1" thickBot="1">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -1992,13 +2001,13 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
@@ -2020,28 +2029,28 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="14">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="49"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="14">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -2050,12 +2059,12 @@
       <c r="K14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="14">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
       <c r="E15" s="32"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -2065,34 +2074,34 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="14">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
       <c r="H16" s="5"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="14">
-      <c r="A17" s="37" t="s">
+      <c r="A17" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37" t="s">
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
@@ -2675,7 +2684,7 @@
       <c r="H57" s="28"/>
     </row>
     <row r="58" spans="1:8" ht="15" thickTop="1">
-      <c r="A58" s="39"/>
+      <c r="A58" s="36"/>
       <c r="B58" s="30"/>
       <c r="C58" s="30"/>
       <c r="D58" s="30"/>
@@ -2685,7 +2694,7 @@
       <c r="H58" s="30"/>
     </row>
     <row r="59" spans="1:8" ht="14">
-      <c r="A59" s="40"/>
+      <c r="A59" s="37"/>
       <c r="B59" s="29"/>
       <c r="C59" s="29"/>
       <c r="D59" s="29"/>
@@ -2695,7 +2704,7 @@
       <c r="H59" s="30"/>
     </row>
     <row r="60" spans="1:8" ht="14">
-      <c r="A60" s="40"/>
+      <c r="A60" s="37"/>
       <c r="B60" s="29"/>
       <c r="C60" s="29"/>
       <c r="D60" s="29"/>
@@ -2705,7 +2714,7 @@
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:8" ht="14">
-      <c r="A61" s="40"/>
+      <c r="A61" s="37"/>
       <c r="B61" s="29"/>
       <c r="C61" s="29"/>
       <c r="D61" s="29"/>
@@ -2716,6 +2725,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A16:G16"/>
@@ -2726,14 +2743,6 @@
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="E17:I17"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A6:H6"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A3:H3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>